<commit_message>
push all updates (3/2)
</commit_message>
<xml_diff>
--- a/Study_Design_LCA_lin copy.xlsx
+++ b/Study_Design_LCA_lin copy.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christinakamis/Documents/DukeSociology/Dissertation/SimulationStudy/LCA_Linear_growth/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E10C2BA-FAE5-B64A-BB83-21F0F4543DE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A71244D-3CA5-4F4C-8AB1-3120C75CADE6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4640" yWindow="740" windowWidth="25000" windowHeight="15920" xr2:uid="{55C899D7-5341-6646-9AD2-6105D9DE32D5}"/>
+    <workbookView xWindow="1780" yWindow="460" windowWidth="22780" windowHeight="15920" activeTab="4" xr2:uid="{55C899D7-5341-6646-9AD2-6105D9DE32D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
     <sheet name="Consistent" sheetId="2" r:id="rId2"/>
     <sheet name="Changing" sheetId="3" r:id="rId3"/>
+    <sheet name="One-Step Files that didn't run" sheetId="4" r:id="rId4"/>
+    <sheet name="Multi-Step that didn't run" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="106">
   <si>
     <t>Data Conditions</t>
   </si>
@@ -70,9 +72,6 @@
     <t>Proportion of smaller class (x3)</t>
   </si>
   <si>
-    <t xml:space="preserve">Factor </t>
-  </si>
-  <si>
     <t>Levels</t>
   </si>
   <si>
@@ -82,39 +81,6 @@
     <t>Sample size (x3)</t>
   </si>
   <si>
-    <t>Class 2 prop</t>
-  </si>
-  <si>
-    <t>(small) 500</t>
-  </si>
-  <si>
-    <t>(large) 2000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Class separation </t>
-  </si>
-  <si>
-    <t>low</t>
-  </si>
-  <si>
-    <t>medium</t>
-  </si>
-  <si>
-    <t>high</t>
-  </si>
-  <si>
-    <t>(medium) 1000</t>
-  </si>
-  <si>
-    <t>(medium) .15</t>
-  </si>
-  <si>
-    <t>(equal) .5</t>
-  </si>
-  <si>
-    <t>(med-eq) .30</t>
-  </si>
-  <si>
     <t xml:space="preserve">Parameter </t>
   </si>
   <si>
@@ -127,21 +93,12 @@
     <t>Mean (I)</t>
   </si>
   <si>
-    <t>var(I)</t>
-  </si>
-  <si>
-    <t>var (S)</t>
-  </si>
-  <si>
     <t>Mean (S)</t>
   </si>
   <si>
     <t>Cov(I,S)</t>
   </si>
   <si>
-    <t>Resid</t>
-  </si>
-  <si>
     <t>approximately 5:1 (see, e.g., Depaoli, 2013; Liu, 2012).</t>
   </si>
   <si>
@@ -154,9 +111,6 @@
     <t>Class 2</t>
   </si>
   <si>
-    <t xml:space="preserve">*in order to test the naïve three-step you would have to assume that the variances are equal across classes </t>
-  </si>
-  <si>
     <t>Low, decreasing (Larger class)</t>
   </si>
   <si>
@@ -223,9 +177,6 @@
     <t>One for each condition*1000</t>
   </si>
   <si>
-    <t>One for each condition*1000*(methods (+1 for first step of all multi step))</t>
-  </si>
-  <si>
     <t>One for each condition*1000*2 (One-Step and first step of multi step)</t>
   </si>
   <si>
@@ -272,25 +223,151 @@
   </si>
   <si>
     <t>49 GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R Script for combining &amp; analyzing fit for 1 and 3 class models </t>
+  </si>
+  <si>
+    <t>One for each condition*3 measures (average parameter values, rmse, absolute bias)</t>
+  </si>
+  <si>
+    <t>TXT files of parameter results for each run, organized by condition &amp; method</t>
+  </si>
+  <si>
+    <t>One for each conditions*#methods</t>
+  </si>
+  <si>
+    <t>One for each condition*1000*(#methods (+1 for first step of all multi step))</t>
+  </si>
+  <si>
+    <t>#methods (+1 for first step of all multi step)</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Solution</t>
+  </si>
+  <si>
+    <t>Fixed?</t>
+  </si>
+  <si>
+    <t>inp-sim-data-s-med-low673.inp</t>
+  </si>
+  <si>
+    <t>inp-sim-data-s-med-low736.inp</t>
+  </si>
+  <si>
+    <t>inp-sim-data-s-med-low843.inp</t>
+  </si>
+  <si>
+    <t>inp-sim-data-s-med-low848.inp</t>
+  </si>
+  <si>
+    <t>inp-sim-data-s-med-low961.inp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">only one latent class defined </t>
+  </si>
+  <si>
+    <t xml:space="preserve">for right now--going to just not count these in RMSE but make a note </t>
+  </si>
+  <si>
+    <t>These same did not run for 3-Step method</t>
+  </si>
+  <si>
+    <t>These same did not run for ML method</t>
+  </si>
+  <si>
+    <t>"N" has no variance</t>
+  </si>
+  <si>
+    <t>Nominal variable N contains less than 2 categories.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multi-step Methods </t>
+  </si>
+  <si>
+    <t>These same ran, but did not converge for BCH</t>
+  </si>
+  <si>
+    <t>3 perturbed starting value run(s) did not converge.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Two-step was able to run these fine </t>
+  </si>
+  <si>
+    <t>Var(I)</t>
+  </si>
+  <si>
+    <t>Var (S)</t>
+  </si>
+  <si>
+    <t>Residual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Condition </t>
+  </si>
+  <si>
+    <t>Class Size (% of respondents in Class 2)</t>
+  </si>
+  <si>
+    <t>Small (500)</t>
+  </si>
+  <si>
+    <t>Medium (1,000)</t>
+  </si>
+  <si>
+    <t>Large (2,000)</t>
+  </si>
+  <si>
+    <t>Unequal (15%)</t>
+  </si>
+  <si>
+    <t>Slightly unequal  (30%)</t>
+  </si>
+  <si>
+    <t>Equal (50%)</t>
+  </si>
+  <si>
+    <t>Low (.754)</t>
+  </si>
+  <si>
+    <t>Class separation (threshold parameter)</t>
+  </si>
+  <si>
+    <t>Medium (1.254)</t>
+  </si>
+  <si>
+    <t>High (1.750)</t>
+  </si>
+  <si>
+    <t>*in order to test the naïve three-step you would have to assume that the variances are equal across classes  (NO LONGER TRUE--can use multigroup analyses to do this)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Homoskedastic </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heteroskedastic </t>
+  </si>
+  <si>
+    <t xml:space="preserve">*THIS NEED TO BE RECORDED AGAIN AFTER RUNS OF NEW SIMULATED DATA </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -309,16 +386,56 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times Roman"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times Roman"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times Roman"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -326,22 +443,67 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,6 +536,39 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Growth for Class 1</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>&amp; 2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -414,7 +609,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Consistent!$B$14</c:f>
+              <c:f>Consistent!$B$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -437,7 +632,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Consistent!$A$15:$A$18</c:f>
+              <c:f>Consistent!$A$17:$A$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -458,7 +653,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Consistent!$B$15:$B$18</c:f>
+              <c:f>Consistent!$B$17:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -489,7 +684,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Consistent!$C$14</c:f>
+              <c:f>Consistent!$C$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -512,7 +707,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Consistent!$A$15:$A$18</c:f>
+              <c:f>Consistent!$A$17:$A$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -533,7 +728,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Consistent!$C$15:$C$18</c:f>
+              <c:f>Consistent!$C$17:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1323,13 +1518,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>768350</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>387350</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>158750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1655,471 +1850,505 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B429AD-E3CE-6840-8A17-4A1355F94BC7}">
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="10"/>
+    <col min="11" max="12" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:13">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="G1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="G1" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
       <c r="L1" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="M1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="G2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="G2" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="G3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="G3" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
       <c r="L3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:13">
+      <c r="A4" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="G4" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="G4" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
       <c r="L4">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="M4" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="G5" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="G5" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
       <c r="L5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:13">
+      <c r="A6" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="G6" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6">
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="G6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1">
+        <f>27*5</f>
+        <v>135</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="G7" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7">
+        <f>27*3</f>
+        <v>81</v>
+      </c>
+      <c r="M7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="G8" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8">
+        <v>2</v>
+      </c>
+      <c r="M8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="G9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="21"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="G11" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="G12" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="1">
         <v>27</v>
       </c>
-      <c r="M6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="G7" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7">
-        <v>2</v>
-      </c>
-      <c r="M7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="G9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="G10" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10">
+      <c r="M12" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="G13" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="1">
         <v>27</v>
       </c>
-      <c r="M10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="G11" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="G12" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12">
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="G14" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="3">
         <f>27*1000</f>
         <v>27000</v>
       </c>
-      <c r="M12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="G13" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13">
-        <f>L12*6</f>
+      <c r="M14" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="G15" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="1">
+        <f>L14*6</f>
         <v>162000</v>
       </c>
-      <c r="M13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="G14" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14">
-        <f>L12*6</f>
+      <c r="M15" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="G16" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="1">
+        <f>L14*6</f>
         <v>162000</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="G15" t="s">
-        <v>73</v>
-      </c>
-      <c r="L15">
-        <f>L11*1000</f>
+      <c r="M16" s="1"/>
+    </row>
+    <row r="17" spans="7:15">
+      <c r="G17" t="s">
+        <v>56</v>
+      </c>
+      <c r="L17" s="1">
+        <f>L13*1000</f>
         <v>27000</v>
       </c>
-      <c r="M15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="G16" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16">
+      <c r="M17" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="7:15">
+      <c r="G18" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="1">
         <f>27*1000*2</f>
         <v>54000</v>
       </c>
-      <c r="M16" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="7:15" x14ac:dyDescent="0.2">
-      <c r="G17" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17">
-        <f>L12*2</f>
+      <c r="M18" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="7:15">
+      <c r="G19" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="1">
+        <f>L14*2</f>
         <v>54000</v>
       </c>
-    </row>
-    <row r="18" spans="7:15" x14ac:dyDescent="0.2">
-      <c r="G18" s="2" t="s">
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="7:15">
+      <c r="G20" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="1">
+        <f>L14*2</f>
+        <v>54000</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="7:15">
+      <c r="G21" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="1">
+        <f>L14*2</f>
+        <v>54000</v>
+      </c>
+      <c r="M21" s="1"/>
+    </row>
+    <row r="25" spans="7:15">
+      <c r="L25" t="s">
+        <v>49</v>
+      </c>
+      <c r="M25" t="s">
+        <v>50</v>
+      </c>
+      <c r="N25" t="s">
+        <v>54</v>
+      </c>
+      <c r="O25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="7:15">
+      <c r="K26" t="s">
+        <v>51</v>
+      </c>
+      <c r="L26">
+        <f>L12+L15+L18+L20</f>
+        <v>270027</v>
+      </c>
+      <c r="M26">
+        <f>L13+L16+L19+L21</f>
+        <v>270027</v>
+      </c>
+      <c r="N26">
+        <f>L14</f>
+        <v>27000</v>
+      </c>
+      <c r="O26">
+        <f>L17</f>
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="27" spans="7:15">
+      <c r="K27" t="s">
+        <v>52</v>
+      </c>
+      <c r="L27">
+        <v>4</v>
+      </c>
+      <c r="M27">
+        <v>20</v>
+      </c>
+      <c r="N27">
+        <v>217</v>
+      </c>
+      <c r="O27">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="28" spans="7:15">
+      <c r="K28" t="s">
+        <v>58</v>
+      </c>
+      <c r="L28">
+        <f>L26*L27</f>
+        <v>1080108</v>
+      </c>
+      <c r="M28">
+        <f t="shared" ref="M28" si="0">M26*M27</f>
+        <v>5400540</v>
+      </c>
+      <c r="N28">
+        <f>N26*N27</f>
+        <v>5859000</v>
+      </c>
+      <c r="O28">
+        <f>O26*O27</f>
+        <v>20790000</v>
+      </c>
+    </row>
+    <row r="31" spans="7:15">
+      <c r="K31" t="s">
+        <v>57</v>
+      </c>
+      <c r="L31">
+        <f>SUM(L28:O28)</f>
+        <v>33129648</v>
+      </c>
+      <c r="M31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="7:15">
+      <c r="K32" t="s">
         <v>60</v>
       </c>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18">
-        <f>L12*2</f>
-        <v>54000</v>
-      </c>
-      <c r="M18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="7:15" x14ac:dyDescent="0.2">
-      <c r="G19" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19">
-        <f>L12*2</f>
-        <v>54000</v>
-      </c>
-    </row>
-    <row r="24" spans="7:15" x14ac:dyDescent="0.2">
-      <c r="L24" t="s">
-        <v>66</v>
-      </c>
-      <c r="M24" t="s">
-        <v>67</v>
-      </c>
-      <c r="N24" t="s">
-        <v>71</v>
-      </c>
-      <c r="O24" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="7:15" x14ac:dyDescent="0.2">
-      <c r="K25" t="s">
-        <v>68</v>
-      </c>
-      <c r="L25">
-        <f>L10+L13+L16+L18</f>
-        <v>270027</v>
-      </c>
-      <c r="M25">
-        <f>L11+L14+L17+L19</f>
-        <v>270027</v>
-      </c>
-      <c r="N25">
-        <f>L12</f>
-        <v>27000</v>
-      </c>
-      <c r="O25">
-        <f>L15</f>
-        <v>27000</v>
-      </c>
-    </row>
-    <row r="26" spans="7:15" x14ac:dyDescent="0.2">
-      <c r="K26" t="s">
-        <v>69</v>
-      </c>
-      <c r="L26">
-        <v>4</v>
-      </c>
-      <c r="M26">
-        <v>20</v>
-      </c>
-      <c r="N26">
-        <v>217</v>
-      </c>
-      <c r="O26">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="27" spans="7:15" x14ac:dyDescent="0.2">
-      <c r="K27" t="s">
-        <v>75</v>
-      </c>
-      <c r="L27">
-        <f>L25*L26</f>
-        <v>1080108</v>
-      </c>
-      <c r="M27">
-        <f t="shared" ref="M27:O27" si="0">M25*M26</f>
-        <v>5400540</v>
-      </c>
-      <c r="N27">
-        <f t="shared" si="0"/>
-        <v>5859000</v>
-      </c>
-      <c r="O27">
-        <f t="shared" si="0"/>
-        <v>20790000</v>
-      </c>
-    </row>
-    <row r="30" spans="7:15" x14ac:dyDescent="0.2">
-      <c r="K30" t="s">
-        <v>74</v>
-      </c>
-      <c r="L30">
-        <f>SUM(L27:O27)</f>
-        <v>33129648</v>
-      </c>
-      <c r="M30" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="31" spans="7:15" x14ac:dyDescent="0.2">
-      <c r="K31" t="s">
-        <v>77</v>
-      </c>
-      <c r="M31" t="s">
-        <v>78</v>
+      <c r="M32" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="G16:K16"/>
-    <mergeCell ref="G17:K17"/>
-    <mergeCell ref="G18:K18"/>
-    <mergeCell ref="G19:K19"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="G13:K13"/>
-    <mergeCell ref="G14:K14"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A7:E7"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A15:E15"/>
@@ -2128,21 +2357,24 @@
     <mergeCell ref="G3:K3"/>
     <mergeCell ref="G4:K4"/>
     <mergeCell ref="G5:K5"/>
-    <mergeCell ref="G6:K6"/>
     <mergeCell ref="G7:K7"/>
     <mergeCell ref="G8:K8"/>
+    <mergeCell ref="G10:K10"/>
     <mergeCell ref="A8:E8"/>
     <mergeCell ref="A9:E9"/>
     <mergeCell ref="A10:E10"/>
     <mergeCell ref="A11:E11"/>
     <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="G19:K19"/>
+    <mergeCell ref="G20:K20"/>
+    <mergeCell ref="G21:K21"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="G14:K14"/>
+    <mergeCell ref="G15:K15"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="G18:K18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2150,164 +2382,252 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{610BBED1-E062-6A45-BBA8-985DBA0573D0}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="11"/>
+    <col min="2" max="3" width="14.33203125" style="11" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="11"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3">
+    <row r="1" spans="1:7">
+      <c r="B1" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="B2" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="12" customFormat="1" ht="68">
+      <c r="A3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="17">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="C4" s="17">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4">
+      <c r="E4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="17">
+        <v>3</v>
+      </c>
+      <c r="G4" s="17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="17">
         <v>-0.25</v>
       </c>
-      <c r="C4">
+      <c r="C5" s="17">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5">
+      <c r="E5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="17">
+        <v>-0.25</v>
+      </c>
+      <c r="G5" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="17">
         <v>2</v>
       </c>
-      <c r="C5">
+      <c r="C6" s="17">
         <v>2</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6">
+      <c r="E6" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="F6" s="17">
+        <v>1</v>
+      </c>
+      <c r="G6" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="17">
         <v>0.4</v>
       </c>
-      <c r="C6">
+      <c r="C7" s="17">
         <v>0.4</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7">
+      <c r="E7" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7" s="17">
+        <v>0.2</v>
+      </c>
+      <c r="G7" s="17">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="17">
         <v>0.5</v>
       </c>
-      <c r="C7">
+      <c r="C8" s="17">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8">
+      <c r="E8" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="17">
+        <v>0.3</v>
+      </c>
+      <c r="G8" s="17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="17">
         <v>1</v>
       </c>
-      <c r="C8">
+      <c r="C9" s="17">
         <v>1</v>
       </c>
-      <c r="E8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="E9" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F9" s="17">
+        <v>0.7</v>
+      </c>
+      <c r="G9" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="11">
         <v>0</v>
       </c>
-      <c r="B15">
-        <f>B3</f>
+      <c r="B17" s="11">
+        <f>B4</f>
         <v>3</v>
       </c>
-      <c r="C15">
-        <f>C3</f>
+      <c r="C17" s="11">
+        <f>C4</f>
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16">
+    <row r="18" spans="1:3">
+      <c r="A18" s="11">
         <v>1</v>
       </c>
-      <c r="B16">
-        <f>3+ (A16*-0.25)</f>
+      <c r="B18" s="11">
+        <f>3+ (A18*-0.25)</f>
         <v>2.75</v>
       </c>
-      <c r="C16">
-        <f>6+(A16*1)</f>
+      <c r="C18" s="11">
+        <f>6+(A18*1)</f>
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17">
+    <row r="19" spans="1:3">
+      <c r="A19" s="11">
         <v>2</v>
       </c>
-      <c r="B17">
-        <f t="shared" ref="B17:B18" si="0">3+ (A17*-0.25)</f>
+      <c r="B19" s="11">
+        <f t="shared" ref="B19:B20" si="0">3+ (A19*-0.25)</f>
         <v>2.5</v>
       </c>
-      <c r="C17">
-        <f t="shared" ref="C17:C18" si="1">6+(A17*1)</f>
+      <c r="C19" s="11">
+        <f t="shared" ref="C19:C20" si="1">6+(A19*1)</f>
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18">
+    <row r="20" spans="1:3">
+      <c r="A20" s="11">
         <v>3</v>
       </c>
-      <c r="B18">
+      <c r="B20" s="11">
         <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
-      <c r="C18">
+      <c r="C20" s="11">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
@@ -2320,74 +2640,343 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AC963B6-F2A5-E849-8B5D-A6C4543E9FCC}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B11" sqref="B11:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="25.1640625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="32.5" style="13" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="17">
+      <c r="A1" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17">
+      <c r="A2" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="12"/>
+    </row>
+    <row r="3" spans="1:2" s="9" customFormat="1" ht="17">
+      <c r="A3" s="19"/>
+      <c r="B3" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17">
+      <c r="A4" s="19"/>
+      <c r="B4" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17">
+      <c r="A5" s="19"/>
+      <c r="B5" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="34">
+      <c r="A6" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="12"/>
+    </row>
+    <row r="7" spans="1:2" ht="17">
+      <c r="A7" s="19"/>
+      <c r="B7" s="12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="17">
+      <c r="A8" s="19"/>
+      <c r="B8" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" s="9" customFormat="1" ht="17">
+      <c r="A9" s="19"/>
+      <c r="B9" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="34">
+      <c r="A10" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="12"/>
+    </row>
+    <row r="11" spans="1:2" ht="17">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="17">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="17">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7658605-F1EE-7047-9AAA-5BEA41563739}">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="36.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>68</v>
+      </c>
+      <c r="B1" t="s">
+        <v>69</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+      <c r="D1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F9739A6-0192-7747-99CD-0702A2F6E595}">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="40.33203125" customWidth="1"/>
+    <col min="2" max="2" width="43.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="20" customFormat="1">
+      <c r="A1" s="20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
       <c r="C3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C10" t="s">
-        <v>21</v>
+        <v>74</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19">
+        <f>1000-5</f>
+        <v>995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>